<commit_message>
Prepare for new results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelocysneiros/git/Anomaly-Detection-IoT23-marcelovca90/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\git\Anomaly-Detection-IoT23-marcelovca90\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71B3258-E3DD-5947-BB7E-9FDDAF355BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F39D3-9EED-4D5C-AF10-2983958A913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{AE7DCEB3-74DD-A143-ABAA-FD16B9429F42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{AE7DCEB3-74DD-A143-ABAA-FD16B9429F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Naive Bayes</t>
   </si>
@@ -69,34 +69,46 @@
 (2021-05)</t>
   </si>
   <si>
-    <t>0,67 (?)</t>
-  </si>
-  <si>
-    <t>0,69 (RBF)</t>
-  </si>
-  <si>
     <t>ANN</t>
   </si>
   <si>
     <t>AdaBoost</t>
   </si>
   <si>
-    <t>0,6751 (sigmoid)</t>
-  </si>
-  <si>
-    <t>0,6900 (RBF)</t>
-  </si>
-  <si>
-    <t>0,7975 (linear)</t>
-  </si>
-  <si>
-    <t>??? (poly)</t>
+    <t>Aragão
+(2022-03)</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>0,6700
+(kernel=?)</t>
+  </si>
+  <si>
+    <t>0,6900
+(kernel=RBF)</t>
+  </si>
+  <si>
+    <t>0,7975
+(kernel=linear)</t>
+  </si>
+  <si>
+    <t>?,????
+(kernel=poly)</t>
+  </si>
+  <si>
+    <t>0,6751
+(kernel=sigmoid)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -178,38 +190,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,160 +560,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821EDE15-2CB5-8A49-BD3B-557A5FA46064}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="6"/>
+    <col min="3" max="3" width="21.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.87</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.69010000000000005</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5">
-        <v>0.87</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5">
-        <v>0.69010000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="7">
         <v>0.23</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="7">
         <v>0.3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="1">
         <v>0.69230000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.73</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.73060000000000003</v>
+      </c>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" s="18">
+        <v>0.66</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
-        <v>0.73</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.73060000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.69350000000000001</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11">
         <v>0.69340000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.995</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.69340000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.995</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="D13" s="11">
         <v>0.73029999999999995</v>
       </c>
+      <c r="E13" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
+  <mergeCells count="7">
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>